<commit_message>
active case tab test case added
</commit_message>
<xml_diff>
--- a/cypress/downloads/download.xlsx
+++ b/cypress/downloads/download.xlsx
@@ -130,16 +130,16 @@
     <t>Triaged</t>
   </si>
   <si>
-    <t>SV22-550</t>
+    <t>SV22-578</t>
   </si>
   <si>
-    <t>SV22-551</t>
+    <t>SV22-579</t>
   </si>
   <si>
-    <t>SV22-552</t>
+    <t>SV22-580</t>
   </si>
   <si>
-    <t>SV22-553</t>
+    <t>SV22-581</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
add create new client test case
</commit_message>
<xml_diff>
--- a/cypress/downloads/download.xlsx
+++ b/cypress/downloads/download.xlsx
@@ -130,16 +130,16 @@
     <t>Triaged</t>
   </si>
   <si>
-    <t>SV22-578</t>
+    <t>SV22-611</t>
   </si>
   <si>
-    <t>SV22-579</t>
+    <t>SV22-612</t>
   </si>
   <si>
-    <t>SV22-580</t>
+    <t>SV22-613</t>
   </si>
   <si>
-    <t>SV22-581</t>
+    <t>SV22-614</t>
   </si>
 </sst>
 </file>

</xml_diff>